<commit_message>
update analytics page with new data and fixed bugs on analytics page
</commit_message>
<xml_diff>
--- a/app/data/csvOut.xlsx
+++ b/app/data/csvOut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\BN3PEPF0000C9A4\EXCELCNV\fed8fdbd-b197-4cb1-b722-9bd8efd28681\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unomail-my.sharepoint.com/personal/mkrupa_unomaha_edu/Documents/CAPSTONE/agro-ai/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F550B3E-374E-4759-8066-E10D4C7DEA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{5F550B3E-374E-4759-8066-E10D4C7DEA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5DE5EA4-1EB3-CF46-976D-6BB6CE7D5835}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{A8D73CEF-C045-4B7B-AFBD-CC9706F60451}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15480" windowHeight="11640" xr2:uid="{A8D73CEF-C045-4B7B-AFBD-CC9706F60451}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -587,68 +587,68 @@
     <t>IMG_6593.Jpeg</t>
   </si>
   <si>
-    <t>IMG_6599 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6600 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6604 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6631 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6632 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6634 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6645 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6657 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6662 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6663 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6673 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6682 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6700 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6705 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6706 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6716 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6719 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6727 - Copy.Jpeg</t>
-  </si>
-  <si>
-    <t>IMG_6729 - Copy.Jpeg</t>
+    <t>IMG_6682.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6599.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6600.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6604.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6631.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6632.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6634.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6645.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6657.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6662.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6663.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6673.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6700.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6705.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6706.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6716.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6719.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6727.Jpeg</t>
+  </si>
+  <si>
+    <t>IMG_6729.Jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1187,9 +1187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1227,7 +1227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1333,7 +1333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1475,7 +1475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1485,11 +1485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D910D22-3E97-43D2-9134-F69F5B8BF318}">
   <dimension ref="A1:Q200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1595,7 +1597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1807,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1860,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1966,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2019,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2072,7 +2074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2125,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2178,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2284,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2390,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2496,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2549,7 +2551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2602,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2655,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2708,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2761,7 +2763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2814,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2867,7 +2869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2920,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2973,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3026,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3079,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3132,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -3238,7 +3240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3344,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3397,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3450,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3503,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3556,7 +3558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3609,7 +3611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3715,7 +3717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3768,7 +3770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3874,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3980,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -4033,7 +4035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -4086,7 +4088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -4245,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -4298,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -4351,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -4404,7 +4406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -4457,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -4510,7 +4512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -4563,7 +4565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -4616,7 +4618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -4669,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -4775,7 +4777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -4828,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -4881,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -4934,7 +4936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -4987,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -5040,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -5093,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -5146,7 +5148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -5199,7 +5201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -5252,7 +5254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -5305,7 +5307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -5358,7 +5360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -5411,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -5464,7 +5466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -5570,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -5623,7 +5625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -5676,7 +5678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -5729,7 +5731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -5782,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -5835,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -5888,7 +5890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -5941,7 +5943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -5994,7 +5996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -6047,7 +6049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -6100,7 +6102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -6153,7 +6155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -6206,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -6259,7 +6261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -6312,7 +6314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -6365,7 +6367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -6418,7 +6420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -6471,7 +6473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -6524,7 +6526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -6577,7 +6579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -6630,7 +6632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -6683,7 +6685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -6736,7 +6738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -6789,7 +6791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -6842,7 +6844,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -6895,7 +6897,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -6948,7 +6950,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -7001,7 +7003,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -7054,7 +7056,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -7107,7 +7109,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>108</v>
       </c>
@@ -7160,7 +7162,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -7213,7 +7215,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -7266,7 +7268,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -7319,7 +7321,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>112</v>
       </c>
@@ -7372,7 +7374,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -7425,7 +7427,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>114</v>
       </c>
@@ -7478,7 +7480,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -7531,7 +7533,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>116</v>
       </c>
@@ -7584,7 +7586,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -7637,7 +7639,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -7690,7 +7692,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>119</v>
       </c>
@@ -7743,7 +7745,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -7796,7 +7798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -7849,7 +7851,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>122</v>
       </c>
@@ -7902,7 +7904,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>123</v>
       </c>
@@ -7955,7 +7957,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -8008,7 +8010,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>125</v>
       </c>
@@ -8061,7 +8063,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>126</v>
       </c>
@@ -8114,7 +8116,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>127</v>
       </c>
@@ -8167,7 +8169,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>128</v>
       </c>
@@ -8220,7 +8222,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>129</v>
       </c>
@@ -8273,7 +8275,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>130</v>
       </c>
@@ -8326,7 +8328,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -8379,7 +8381,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>132</v>
       </c>
@@ -8432,7 +8434,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>133</v>
       </c>
@@ -8485,7 +8487,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>134</v>
       </c>
@@ -8538,7 +8540,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="134" spans="1:17">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>135</v>
       </c>
@@ -8591,7 +8593,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="135" spans="1:17">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>136</v>
       </c>
@@ -8644,7 +8646,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="136" spans="1:17">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>137</v>
       </c>
@@ -8697,7 +8699,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="137" spans="1:17">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -8750,7 +8752,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -8803,7 +8805,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>140</v>
       </c>
@@ -8856,7 +8858,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -8909,7 +8911,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>142</v>
       </c>
@@ -8962,7 +8964,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>143</v>
       </c>
@@ -9015,7 +9017,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>144</v>
       </c>
@@ -9068,7 +9070,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>145</v>
       </c>
@@ -9121,7 +9123,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -9174,7 +9176,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>147</v>
       </c>
@@ -9227,7 +9229,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>148</v>
       </c>
@@ -9280,7 +9282,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -9333,7 +9335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -9386,7 +9388,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>151</v>
       </c>
@@ -9439,7 +9441,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>152</v>
       </c>
@@ -9492,7 +9494,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>153</v>
       </c>
@@ -9545,7 +9547,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -9598,7 +9600,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -9651,7 +9653,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -9704,7 +9706,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -9757,7 +9759,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -9810,7 +9812,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -9863,7 +9865,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -9916,7 +9918,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -9969,7 +9971,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="161" spans="1:17">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -10022,7 +10024,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="162" spans="1:17">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -10075,7 +10077,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="163" spans="1:17">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -10128,7 +10130,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="164" spans="1:17">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -10181,7 +10183,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="165" spans="1:17">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -10234,7 +10236,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="166" spans="1:17">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -10287,7 +10289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="167" spans="1:17">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -10340,7 +10342,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="168" spans="1:17">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -10393,7 +10395,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="169" spans="1:17">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -10446,7 +10448,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="170" spans="1:17">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -10499,7 +10501,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="171" spans="1:17">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -10552,7 +10554,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -10605,7 +10607,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="173" spans="1:17">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -10658,7 +10660,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="174" spans="1:17">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -10711,7 +10713,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="175" spans="1:17">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -10764,7 +10766,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="176" spans="1:17">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -10817,7 +10819,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="177" spans="1:17">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -10870,7 +10872,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="178" spans="1:17">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -10923,7 +10925,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="179" spans="1:17">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -10976,7 +10978,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="180" spans="1:17">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -11029,7 +11031,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="181" spans="1:17">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -11082,9 +11084,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="182" spans="1:17">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B182">
         <v>1.459492E-3</v>
@@ -11135,9 +11137,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="183" spans="1:17">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B183">
         <v>1.4300370000000001E-3</v>
@@ -11188,9 +11190,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="184" spans="1:17">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B184">
         <v>1.517736E-3</v>
@@ -11241,9 +11243,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="185" spans="1:17">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B185">
         <v>1.344163E-3</v>
@@ -11294,9 +11296,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="186" spans="1:17">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B186">
         <v>1.373832E-3</v>
@@ -11347,9 +11349,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="187" spans="1:17">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B187">
         <v>1.527947E-3</v>
@@ -11400,9 +11402,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="188" spans="1:17">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B188">
         <v>1.584423E-3</v>
@@ -11453,9 +11455,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="189" spans="1:17">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B189">
         <v>1.3907629999999999E-3</v>
@@ -11506,9 +11508,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="190" spans="1:17">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B190">
         <v>1.5204839999999999E-3</v>
@@ -11559,9 +11561,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="191" spans="1:17">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B191">
         <v>1.5401950000000001E-3</v>
@@ -11612,9 +11614,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="192" spans="1:17">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B192">
         <v>1.426117E-3</v>
@@ -11665,9 +11667,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="193" spans="1:17">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B193">
         <v>1.495323E-3</v>
@@ -11718,7 +11720,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="194" spans="1:17">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -11771,7 +11773,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="195" spans="1:17">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -11824,7 +11826,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="196" spans="1:17">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -11877,7 +11879,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="197" spans="1:17">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -11930,7 +11932,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="198" spans="1:17">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -11983,7 +11985,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="199" spans="1:17">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -12036,7 +12038,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="200" spans="1:17">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>201</v>
       </c>

</xml_diff>